<commit_message>
Reorganised structure & added links to data points
</commit_message>
<xml_diff>
--- a/src/assets/table_data_CLFV.xlsx
+++ b/src/assets/table_data_CLFV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archibaldruban/Documents/Coding Projects/PHAS0052 - Website/PHAS0052_website/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1879CC72-585B-CC47-ABA7-8408D33DCF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C8E4C1-7DC2-B646-AEB2-9B874462CE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{D410D509-C897-B34B-84AA-51E28B806201}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16040" xr2:uid="{D410D509-C897-B34B-84AA-51E28B806201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="113">
   <si>
     <t>Liverpool</t>
   </si>
@@ -111,6 +111,252 @@
     <t>JINR</t>
   </si>
   <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-0011529246&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149005406&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:J.%20Steinberger</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:T.%20O%E2%80%99Keefe</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-84989002681&amp;origin=inward</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149013077&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-51249195115&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-52449139585&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-0001482815&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149014253&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>Hincks and Pontecorvo</t>
+  </si>
+  <si>
+    <t>Sard and Althaus</t>
+  </si>
+  <si>
+    <t>Steinberger and Lokanathan</t>
+  </si>
+  <si>
+    <t>O'Keefe et al.</t>
+  </si>
+  <si>
+    <t>Berley et al.</t>
+  </si>
+  <si>
+    <t>Ashkin et al.</t>
+  </si>
+  <si>
+    <t>Davis et al.</t>
+  </si>
+  <si>
+    <t>Frankel et al.</t>
+  </si>
+  <si>
+    <t>Crittenden et al.</t>
+  </si>
+  <si>
+    <t>Parker et al.</t>
+  </si>
+  <si>
+    <t>Korenchenko et al.</t>
+  </si>
+  <si>
+    <t>Depommier et al.</t>
+  </si>
+  <si>
+    <t>Povel et al.</t>
+  </si>
+  <si>
+    <t>Bowman et al..</t>
+  </si>
+  <si>
+    <t>Kinnison et al.</t>
+  </si>
+  <si>
+    <t>Bolton et al.</t>
+  </si>
+  <si>
+    <t>Brooks et al.</t>
+  </si>
+  <si>
+    <t>Adam et al.</t>
+  </si>
+  <si>
+    <t>Lagarrigue and Peyrou</t>
+  </si>
+  <si>
+    <t>Steinberger and Wolfe</t>
+  </si>
+  <si>
+    <t>Sard et al.</t>
+  </si>
+  <si>
+    <t>Conversi et al.</t>
+  </si>
+  <si>
+    <t>Conforto et al.</t>
+  </si>
+  <si>
+    <t>Bartley et al.</t>
+  </si>
+  <si>
+    <t>Bryman et al.</t>
+  </si>
+  <si>
+    <t>Badertscher et al.</t>
+  </si>
+  <si>
+    <t>Ahmad et al.</t>
+  </si>
+  <si>
+    <t>Dohmen et al.</t>
+  </si>
+  <si>
+    <t>Eggli</t>
+  </si>
+  <si>
+    <t>Honecker et al.</t>
+  </si>
+  <si>
+    <t>Bertl et al.</t>
+  </si>
+  <si>
+    <t>Lynch et al.</t>
+  </si>
+  <si>
+    <t>Lee and Samios</t>
+  </si>
+  <si>
+    <t>Parker and penman</t>
+  </si>
+  <si>
+    <t>Bellgardt et al.</t>
+  </si>
+  <si>
+    <t>Baranov et al.</t>
+  </si>
+  <si>
+    <t>Bartlett et al.</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-4243523863&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-52449139585&amp;origin=inward</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-84885956626&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-4243604295&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0370269377906979</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-24444479495&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-0000704919&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-4243428379&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://journals.aps.org/prl/abstract/10.1103/PhysRevLett.83.1521</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/0908.2594</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/hep-ex/1107.5547</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:A.%20Lagarrigue</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149019490&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149011448&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-0039854605&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-51649208024&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0031916364904792</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-4243350658&amp;origin=inward</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0375947482900495</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-4243884384&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:S.%20Ahmad</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/037026939391383X</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C5&amp;q=+author%3AS.+Eggli&amp;btnG=</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-0038779802&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1140/epjc/s2006-02582-x</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149015729&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-36149017189&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-51649208457&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:S.%20Korenchenko</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-26744444022&amp;origin=inward&amp;featureToggles=FEATURE_NEW_DOC_DETAILS_EXPORT:1</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0370269384907573</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0550321385903086</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:R.D.%20Bolton</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0550321388904622</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/scholar?q=+author:V.A.%20Baranov</t>
+  </si>
+  <si>
     <t>year</t>
   </si>
   <si>
@@ -121,16 +367,30 @@
   </si>
   <si>
     <t>decay</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,14 +413,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,29 +736,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3397B13-4A84-494B-888C-0DDCD43391DE}">
-  <dimension ref="A2:D49"/>
+  <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="117" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1947</v>
       </c>
@@ -508,8 +777,14 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1948</v>
       </c>
@@ -522,8 +797,14 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1955</v>
       </c>
@@ -536,8 +817,14 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1959</v>
       </c>
@@ -550,8 +837,14 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1959</v>
       </c>
@@ -564,8 +857,14 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1959</v>
       </c>
@@ -578,8 +877,14 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1959</v>
       </c>
@@ -592,8 +897,14 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1960</v>
       </c>
@@ -606,8 +917,14 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1961</v>
       </c>
@@ -620,8 +937,14 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1962</v>
       </c>
@@ -634,8 +957,14 @@
       <c r="D12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1962</v>
       </c>
@@ -648,8 +977,14 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1963</v>
       </c>
@@ -662,8 +997,14 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1964</v>
       </c>
@@ -676,8 +1017,14 @@
       <c r="D15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1971</v>
       </c>
@@ -690,8 +1037,14 @@
       <c r="D16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1977</v>
       </c>
@@ -704,8 +1057,14 @@
       <c r="D17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1977</v>
       </c>
@@ -718,8 +1077,14 @@
       <c r="D18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1979</v>
       </c>
@@ -732,8 +1097,14 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1982</v>
       </c>
@@ -746,8 +1117,14 @@
       <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1986</v>
       </c>
@@ -760,8 +1137,14 @@
       <c r="D21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1999</v>
       </c>
@@ -774,8 +1157,14 @@
       <c r="D22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -788,8 +1177,14 @@
       <c r="D23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -802,8 +1197,14 @@
       <c r="D24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1952</v>
       </c>
@@ -816,8 +1217,14 @@
       <c r="D25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1955</v>
       </c>
@@ -830,8 +1237,14 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1961</v>
       </c>
@@ -844,8 +1257,14 @@
       <c r="D27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1961</v>
       </c>
@@ -858,8 +1277,14 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1962</v>
       </c>
@@ -872,8 +1297,14 @@
       <c r="D29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1964</v>
       </c>
@@ -886,8 +1317,14 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1972</v>
       </c>
@@ -900,8 +1337,14 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1977</v>
       </c>
@@ -914,8 +1357,14 @@
       <c r="D32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1982</v>
       </c>
@@ -928,8 +1377,14 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1988</v>
       </c>
@@ -942,8 +1397,14 @@
       <c r="D34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1993</v>
       </c>
@@ -956,8 +1417,14 @@
       <c r="D35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1995</v>
       </c>
@@ -970,8 +1437,14 @@
       <c r="D36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1996</v>
       </c>
@@ -984,8 +1457,14 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -998,8 +1477,14 @@
       <c r="D38" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1958</v>
       </c>
@@ -1012,8 +1497,14 @@
       <c r="D39" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1959</v>
       </c>
@@ -1026,8 +1517,14 @@
       <c r="D40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1961</v>
       </c>
@@ -1040,8 +1537,14 @@
       <c r="D41" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1962</v>
       </c>
@@ -1054,8 +1557,14 @@
       <c r="D42" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1976</v>
       </c>
@@ -1068,8 +1577,14 @@
       <c r="D43" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1984</v>
       </c>
@@ -1082,8 +1597,14 @@
       <c r="D44" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1984</v>
       </c>
@@ -1096,8 +1617,14 @@
       <c r="D45" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1985</v>
       </c>
@@ -1110,8 +1637,14 @@
       <c r="D46" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1988</v>
       </c>
@@ -1124,8 +1657,14 @@
       <c r="D47" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1988</v>
       </c>
@@ -1138,8 +1677,14 @@
       <c r="D48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1990</v>
       </c>
@@ -1152,8 +1697,21 @@
       <c r="D49" t="s">
         <v>22</v>
       </c>
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{BCB59FF2-7414-0241-B859-8B08F551AED8}"/>
+    <hyperlink ref="F34" r:id="rId2" xr:uid="{42A70641-1A37-1C49-A5A0-4BEC9C7E7A23}"/>
+    <hyperlink ref="F42" r:id="rId3" xr:uid="{A323CE2A-E2A5-A449-94F6-766B29ADECD1}"/>
+    <hyperlink ref="F44" r:id="rId4" xr:uid="{12F23F4F-F050-5847-B4C2-73179D2DA2A5}"/>
+    <hyperlink ref="F45" r:id="rId5" xr:uid="{7016D724-F29E-3B41-88B4-BCA075621DC2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>